<commit_message>
add services for check and download excel file
</commit_message>
<xml_diff>
--- a/StudentAssistant.Backend/Infrastructure/ScheduleFile/scheduleFile.xlsx
+++ b/StudentAssistant.Backend/Infrastructure/ScheduleFile/scheduleFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3840" windowWidth="15480" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="4080" windowWidth="15480" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7345" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7363" uniqueCount="668">
   <si>
     <t>ВТОРНИК</t>
   </si>
@@ -2122,6 +2122,18 @@
   </si>
   <si>
     <t>1,3,5,7 н.Методы сбора экономически значимой информации 11,13 н. Финансовая отчетность предприятия</t>
+  </si>
+  <si>
+    <t>13 н Уголовно-процессуальное право</t>
+  </si>
+  <si>
+    <t>кр 12 н Уголовно-процессуальное право</t>
+  </si>
+  <si>
+    <t>кр 14 н Технологии создания WEB-приложений и WEB-сервисов</t>
+  </si>
+  <si>
+    <t>14 н Технологии создания WEB-приложений и WEB-сервисов</t>
   </si>
 </sst>
 </file>
@@ -4843,10 +4855,10 @@
   <dimension ref="A1:HW93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="EU34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="BV28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="FL40" sqref="FL40"/>
+      <selection pane="bottomRight" activeCell="CG39" sqref="CG39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -7701,21 +7713,29 @@
       <c r="FO6" s="79">
         <v>344</v>
       </c>
-      <c r="FP6" s="108" t="s">
-        <v>524</v>
-      </c>
-      <c r="FQ6" s="3"/>
-      <c r="FR6" s="25"/>
+      <c r="FP6" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="FQ6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="FR6" s="78" t="s">
+        <v>427</v>
+      </c>
       <c r="FS6" s="37">
-        <v>132</v>
-      </c>
-      <c r="FT6" s="108" t="s">
-        <v>524</v>
-      </c>
-      <c r="FU6" s="3"/>
-      <c r="FV6" s="25"/>
+        <v>250</v>
+      </c>
+      <c r="FT6" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="FU6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="FV6" s="78" t="s">
+        <v>427</v>
+      </c>
       <c r="FW6" s="37">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="FY6" s="450"/>
       <c r="FZ6" s="418">
@@ -7730,13 +7750,17 @@
       <c r="GC6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="GD6" s="108" t="s">
-        <v>524</v>
-      </c>
-      <c r="GE6" s="3"/>
-      <c r="GF6" s="25"/>
+      <c r="GD6" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="GE6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="GF6" s="78" t="s">
+        <v>427</v>
+      </c>
       <c r="GG6" s="37">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="GH6" s="85" t="s">
         <v>350</v>
@@ -8677,21 +8701,29 @@
       <c r="FO8" s="166">
         <v>275</v>
       </c>
-      <c r="FP8" s="108" t="s">
-        <v>524</v>
-      </c>
-      <c r="FQ8" s="3"/>
-      <c r="FR8" s="25"/>
+      <c r="FP8" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="FQ8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="FR8" s="78" t="s">
+        <v>427</v>
+      </c>
       <c r="FS8" s="37">
-        <v>132</v>
-      </c>
-      <c r="FT8" s="108" t="s">
-        <v>524</v>
-      </c>
-      <c r="FU8" s="3"/>
-      <c r="FV8" s="25"/>
+        <v>250</v>
+      </c>
+      <c r="FT8" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="FU8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="FV8" s="78" t="s">
+        <v>427</v>
+      </c>
       <c r="FW8" s="37">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="FY8" s="450"/>
       <c r="FZ8" s="418">
@@ -8706,13 +8738,17 @@
       <c r="GC8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="GD8" s="108" t="s">
-        <v>524</v>
-      </c>
-      <c r="GE8" s="3"/>
-      <c r="GF8" s="25"/>
+      <c r="GD8" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="GE8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="GF8" s="78" t="s">
+        <v>427</v>
+      </c>
       <c r="GG8" s="37">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="GH8" s="85" t="s">
         <v>350</v>
@@ -17818,7 +17854,7 @@
         <v>2</v>
       </c>
       <c r="BZ29" s="183" t="s">
-        <v>227</v>
+        <v>666</v>
       </c>
       <c r="CA29" s="61" t="s">
         <v>174</v>
@@ -18682,7 +18718,7 @@
         <v>2</v>
       </c>
       <c r="BZ31" s="183" t="s">
-        <v>227</v>
+        <v>666</v>
       </c>
       <c r="CA31" s="61" t="s">
         <v>174</v>
@@ -21310,10 +21346,18 @@
       <c r="BY37" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="BZ37" s="60"/>
-      <c r="CA37" s="78"/>
-      <c r="CB37" s="78"/>
-      <c r="CC37" s="63"/>
+      <c r="BZ37" s="183" t="s">
+        <v>667</v>
+      </c>
+      <c r="CA37" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="CB37" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="CC37" s="37">
+        <v>246</v>
+      </c>
       <c r="CD37" s="60"/>
       <c r="CE37" s="78"/>
       <c r="CF37" s="78"/>
@@ -21964,14 +22008,22 @@
       <c r="BY39" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="BZ39" s="142"/>
-      <c r="CA39" s="131"/>
-      <c r="CB39" s="131"/>
-      <c r="CC39" s="63"/>
+      <c r="BZ39" s="164" t="s">
+        <v>667</v>
+      </c>
+      <c r="CA39" s="139" t="s">
+        <v>174</v>
+      </c>
+      <c r="CB39" s="131" t="s">
+        <v>226</v>
+      </c>
+      <c r="CC39" s="128">
+        <v>246</v>
+      </c>
       <c r="CD39" s="142"/>
       <c r="CE39" s="131"/>
       <c r="CF39" s="131"/>
-      <c r="CG39" s="63"/>
+      <c r="CG39" s="294"/>
       <c r="CH39" s="220" t="s">
         <v>229</v>
       </c>
@@ -22308,9 +22360,9 @@
       <c r="BY40" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="BZ40" s="29"/>
-      <c r="CA40" s="3"/>
-      <c r="CB40" s="25"/>
+      <c r="BZ40" s="89"/>
+      <c r="CA40" s="74"/>
+      <c r="CB40" s="75"/>
       <c r="CC40" s="38"/>
       <c r="CD40" s="29"/>
       <c r="CE40" s="3"/>
@@ -28700,7 +28752,7 @@
       <c r="HV53" s="25"/>
       <c r="HW53" s="69"/>
     </row>
-    <row r="54" spans="1:231" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:231" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="428"/>
       <c r="B54" s="418">
         <v>2</v>
@@ -29196,7 +29248,7 @@
       <c r="GK54" s="37">
         <v>385</v>
       </c>
-      <c r="GL54" s="222"/>
+      <c r="GL54" s="85"/>
       <c r="GM54" s="308"/>
       <c r="GN54" s="25"/>
       <c r="GO54" s="37"/>
@@ -29673,10 +29725,10 @@
       <c r="GF55" s="78"/>
       <c r="GG55" s="267"/>
       <c r="GH55" s="92"/>
-      <c r="GI55" s="87"/>
-      <c r="GJ55" s="25"/>
-      <c r="GK55" s="88"/>
-      <c r="GL55" s="62"/>
+      <c r="GI55" s="103"/>
+      <c r="GJ55" s="75"/>
+      <c r="GK55" s="104"/>
+      <c r="GL55" s="114"/>
       <c r="GM55" s="3"/>
       <c r="GN55" s="25"/>
       <c r="GO55" s="37"/>
@@ -30690,7 +30742,7 @@
         <v>344</v>
       </c>
       <c r="FP57" s="62" t="s">
-        <v>340</v>
+        <v>665</v>
       </c>
       <c r="FQ57" s="3" t="s">
         <v>89</v>
@@ -30702,7 +30754,7 @@
         <v>350</v>
       </c>
       <c r="FT57" s="62" t="s">
-        <v>340</v>
+        <v>665</v>
       </c>
       <c r="FU57" s="3" t="s">
         <v>89</v>
@@ -30721,7 +30773,7 @@
         <v>2</v>
       </c>
       <c r="GD57" s="62" t="s">
-        <v>340</v>
+        <v>665</v>
       </c>
       <c r="GE57" s="3" t="s">
         <v>89</v>
@@ -31786,7 +31838,7 @@
         <v>344</v>
       </c>
       <c r="FP59" s="62" t="s">
-        <v>340</v>
+        <v>665</v>
       </c>
       <c r="FQ59" s="3" t="s">
         <v>89</v>
@@ -31798,7 +31850,7 @@
         <v>269</v>
       </c>
       <c r="FT59" s="62" t="s">
-        <v>340</v>
+        <v>665</v>
       </c>
       <c r="FU59" s="3" t="s">
         <v>89</v>
@@ -31817,7 +31869,7 @@
         <v>2</v>
       </c>
       <c r="GD59" s="62" t="s">
-        <v>340</v>
+        <v>665</v>
       </c>
       <c r="GE59" s="3" t="s">
         <v>89</v>

</xml_diff>